<commit_message>
New sheet from chris
</commit_message>
<xml_diff>
--- a/Spreadsheets/formats/MultiGP_Double_Elimination_16_pilots.xlsx
+++ b/Spreadsheets/formats/MultiGP_Double_Elimination_16_pilots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Danside FPV\FPVTrackside\bin\x64\Debug\net48\formats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\AppData\Local\FPVTrackside\formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD2F1FB-E14E-43C3-9DD6-38E6DAA08B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7641E07F-3F53-4634-AD68-B8D834D56752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="21735" windowWidth="28800" windowHeight="15345" xr2:uid="{A1B0FD94-EAE6-4FC0-8B13-9A929C6CF73A}"/>
+    <workbookView xWindow="38295" yWindow="0" windowWidth="38610" windowHeight="20985" xr2:uid="{A1B0FD94-EAE6-4FC0-8B13-9A929C6CF73A}"/>
   </bookViews>
   <sheets>
     <sheet name="FPVTrackside" sheetId="1" r:id="rId1"/>
@@ -417,7 +417,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,8 +444,15 @@
       <name val="Segoe UI"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -454,13 +461,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -539,36 +552,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+  <cellXfs count="30">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7171"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -880,7 +905,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,47 +924,47 @@
     <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -950,36 +975,36 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="18">
         <f>B5</f>
         <v>4</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="16" t="e">
+      <c r="D2" s="27"/>
+      <c r="E2" s="7" t="e">
         <f>INDEX(C2:C5,MATCH(3,D2:D5, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="16" t="e">
+      <c r="F2" s="11"/>
+      <c r="G2" s="7" t="e">
         <f>INDEX(E2:E5,MATCH(1,F2:F5, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="16" t="e">
+      <c r="H2" s="11"/>
+      <c r="I2" s="7" t="e">
         <f>INDEX(G2:G5,MATCH(1,H2:H5, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="16" t="e">
+      <c r="J2" s="11"/>
+      <c r="K2" s="7" t="e">
         <f>INDEX(G10:G13,MATCH(3,H10:H13, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="L2" s="17"/>
-      <c r="M2" s="1" t="e">
+      <c r="L2" s="24"/>
+      <c r="M2" s="8" t="e">
         <f>INDEX(G10:G13,MATCH(1,H10:H13, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="N2" s="2"/>
+      <c r="N2" s="16"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -988,36 +1013,36 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="19">
         <f>B8</f>
         <v>7</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="18" t="e">
+      <c r="D3" s="28"/>
+      <c r="E3" s="5" t="e">
         <f>INDEX(C2:C5,MATCH(4,D2:D5, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="18" t="e">
+      <c r="F3" s="12"/>
+      <c r="G3" s="5" t="e">
         <f>INDEX(E2:E5,MATCH(2,F2:F5, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="18" t="e">
+      <c r="H3" s="12"/>
+      <c r="I3" s="5" t="e">
         <f>INDEX(G2:G5,MATCH(2,H2:H5, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="J3" s="19"/>
-      <c r="K3" s="18" t="e">
+      <c r="J3" s="12"/>
+      <c r="K3" s="5" t="e">
         <f>INDEX(G10:G13,MATCH(4,H10:H13, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="L3" s="19"/>
-      <c r="M3" s="3" t="e">
+      <c r="L3" s="25"/>
+      <c r="M3" s="9" t="e">
         <f>INDEX(G10:G13,MATCH(2,H10:H13, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="N3" s="4"/>
+      <c r="N3" s="17"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="b">
@@ -1026,167 +1051,167 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="19">
         <f>B12</f>
         <v>11</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="18" t="e">
+      <c r="D4" s="28"/>
+      <c r="E4" s="5" t="e">
         <f>INDEX(C6:C9,MATCH(3,D6:D9, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="18" t="e">
-        <f>INDEX(E10:E13,MATCH(1,F10:F13, 0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="18" t="e">
+      <c r="F4" s="12"/>
+      <c r="G4" s="5" t="e">
+        <f>INDEX(E6:E9,MATCH(3,F6:F9, 0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H4" s="12"/>
+      <c r="I4" s="5" t="e">
         <f>INDEX(G6:G9,MATCH(1,H6:H9, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="18" t="e">
+      <c r="J4" s="12"/>
+      <c r="K4" s="5" t="e">
         <f>INDEX(I2:I5,MATCH(1,J2:J5, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="L4" s="19"/>
-      <c r="M4" s="3" t="e">
+      <c r="L4" s="12"/>
+      <c r="M4" s="9" t="e">
         <f>INDEX(K2:K5,MATCH(1,L2:L5, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="N4" s="4"/>
+      <c r="N4" s="17"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="20">
         <f>B14</f>
         <v>13</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="20" t="e">
+      <c r="D5" s="29"/>
+      <c r="E5" s="6" t="e">
         <f>INDEX(C6:C9,MATCH(4,D6:D9, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="20" t="e">
-        <f>INDEX(E10:E13,MATCH(2,F10:F13, 0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="20" t="e">
+      <c r="F5" s="13"/>
+      <c r="G5" s="6" t="e">
+        <f>INDEX(E6:E9,MATCH(4,F6:F9, 0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="I5" s="6" t="e">
         <f>INDEX(G6:G9,MATCH(2,H6:H9, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="J5" s="21"/>
-      <c r="K5" s="20" t="e">
+      <c r="J5" s="13"/>
+      <c r="K5" s="6" t="e">
         <f>INDEX(I2:I5,MATCH(2,J2:J5, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="L5" s="21"/>
-      <c r="M5" s="5" t="e">
+      <c r="L5" s="13"/>
+      <c r="M5" s="26" t="e">
         <f>INDEX(K2:K5,MATCH(2,L2:L5, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="N5" s="6"/>
+      <c r="N5" s="21"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="19">
         <f>B4</f>
         <v>3</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="10" t="e">
+      <c r="D6" s="28"/>
+      <c r="E6" s="3" t="e">
         <f>INDEX(C2:C5,MATCH(1,D2:D5, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="18" t="e">
-        <f>INDEX(E6:E9,MATCH(3,F6:F9, 0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H6" s="19"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="5" t="e">
+        <f>INDEX(E10:E13,MATCH(1,F10:F13, 0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="19">
         <f>B7</f>
         <v>6</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="10" t="e">
+      <c r="D7" s="28"/>
+      <c r="E7" s="3" t="e">
         <f>INDEX(C2:C5,MATCH(2,D2:D5, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="18" t="e">
-        <f>INDEX(E6:E9,MATCH(4,F6:F9, 0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H7" s="19"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="5" t="e">
+        <f>INDEX(E10:E13,MATCH(2,F10:F13, 0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="19">
         <f>B11</f>
         <v>10</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="10" t="e">
+      <c r="D8" s="28"/>
+      <c r="E8" s="3" t="e">
         <f>INDEX(C6:C9,MATCH(1,D6:D9, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="18" t="e">
+      <c r="F8" s="10"/>
+      <c r="G8" s="5" t="e">
         <f>INDEX(E14:E17,MATCH(3,F14:F17, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="H8" s="19"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="20">
         <f>B15</f>
         <v>14</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="12" t="e">
+      <c r="D9" s="29"/>
+      <c r="E9" s="4" t="e">
         <f>INDEX(C6:C9,MATCH(2,D6:D9, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="20" t="e">
+      <c r="F9" s="14"/>
+      <c r="G9" s="6" t="e">
         <f>INDEX(E14:E17,MATCH(4,F14:F17, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="H9" s="21"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>9</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="18">
         <f>B3</f>
         <v>2</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="16" t="e">
+      <c r="D10" s="27"/>
+      <c r="E10" s="7" t="e">
         <f>INDEX(C10:C13,MATCH(3,D10:D13, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="8" t="e">
+      <c r="F10" s="11"/>
+      <c r="G10" s="2" t="e">
         <f>INDEX(E6:E9,MATCH(1,F6:F9, 0))</f>
         <v>#N/A</v>
       </c>
@@ -1196,121 +1221,121 @@
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="19">
         <f>B6</f>
         <v>5</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="18" t="e">
+      <c r="D11" s="28"/>
+      <c r="E11" s="5" t="e">
         <f>INDEX(C10:C13,MATCH(4,D10:D13, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="10" t="e">
+      <c r="F11" s="12"/>
+      <c r="G11" s="3" t="e">
         <f>INDEX(E6:E9,MATCH(2,F6:F9, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="H11" s="14"/>
+      <c r="H11" s="23"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="19">
         <f>B10</f>
         <v>9</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="18" t="e">
+      <c r="D12" s="28"/>
+      <c r="E12" s="5" t="e">
         <f>INDEX(C14:C17,MATCH(3,D14:D17, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="10" t="e">
+      <c r="F12" s="12"/>
+      <c r="G12" s="3" t="e">
         <f>INDEX(E14:E17,MATCH(1,F14:F17, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="H12" s="14"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="20">
         <f>B16</f>
         <v>15</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="20" t="e">
+      <c r="D13" s="29"/>
+      <c r="E13" s="6" t="e">
         <f>INDEX(C14:C17,MATCH(4,D14:D17, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="12" t="e">
+      <c r="F13" s="13"/>
+      <c r="G13" s="4" t="e">
         <f>INDEX(E14:E17,MATCH(2,F14:F17, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="H13" s="15"/>
+      <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>13</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="18">
         <f>B2</f>
         <v>1</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="8" t="e">
+      <c r="D14" s="27"/>
+      <c r="E14" s="2" t="e">
         <f>INDEX(C10:C13,MATCH(1,D10:D13, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="F14" s="22"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>14</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="19">
         <f>B9</f>
         <v>8</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="10" t="e">
+      <c r="D15" s="28"/>
+      <c r="E15" s="3" t="e">
         <f>INDEX(C10:C13,MATCH(2,D10:D13, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="F15" s="14"/>
+      <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>15</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="19">
         <f>B13</f>
         <v>12</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="10" t="e">
+      <c r="D16" s="28"/>
+      <c r="E16" s="3" t="e">
         <f>INDEX(C14:C17,MATCH(1,D14:D17, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="F16" s="14"/>
+      <c r="F16" s="10"/>
     </row>
     <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>16</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="20">
         <f>B17</f>
         <v>16</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="12" t="e">
+      <c r="D17" s="29"/>
+      <c r="E17" s="4" t="e">
         <f>INDEX(C14:C17,MATCH(2,D14:D17, 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="F17" s="15"/>
+      <c r="F17" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>